<commit_message>
Changes in the Manage Drivers Test Page
</commit_message>
<xml_diff>
--- a/test/data/TestData.xlsx
+++ b/test/data/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximo\Desktop\Spectron test\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karen\Desktop\Repo\Spectron test\QA_Capstone_React\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE20F3D5-7978-4082-87F2-9076641A980B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142919D4-4941-496C-A9BD-CFA8D793DCD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3330" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2700" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>TestCase</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Select Branch</t>
   </si>
   <si>
-    <t>AdminUser</t>
-  </si>
-  <si>
     <t>Capstone Main Menu</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>SecondaryUser</t>
-  </si>
-  <si>
     <t>Pages where displayed</t>
   </si>
   <si>
@@ -118,7 +112,16 @@
     <t>PhoEnix</t>
   </si>
   <si>
-    <t>Johns Smithfffda</t>
+    <t>CapstoneUser</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>WsUser</t>
+  </si>
+  <si>
+    <t>Johns Smith123</t>
   </si>
 </sst>
 </file>
@@ -504,19 +507,19 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,18 +536,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
@@ -553,27 +556,27 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -590,46 +593,46 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
-    <col min="4" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -645,54 +648,54 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D14" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -711,36 +714,36 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>

</xml_diff>